<commit_message>
updating progress on denove inference
</commit_message>
<xml_diff>
--- a/documents/tables/set_1_metadata.xlsx
+++ b/documents/tables/set_1_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Dala\documentos\phd\Duke\lutzoniLab\genomes\nostoc\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/titus/Dropbox (Duke Bio_Ea)/Carlos/PhD/Projects/cyanolichen_holobiome/documents/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AF26A4-ECA4-44FF-9DAD-58868016C501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B07193-3B73-FA42-931B-4C8051B4D49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D54A0E47-B65D-4016-AF98-0E69F3F62F9D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{D54A0E47-B65D-4016-AF98-0E69F3F62F9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="548">
   <si>
     <t>taxon_name</t>
   </si>
@@ -1677,6 +1677,9 @@
   </si>
   <si>
     <t>lichen</t>
+  </si>
+  <si>
+    <t>macrozamia</t>
   </si>
 </sst>
 </file>
@@ -2048,24 +2051,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB05894-1E4B-404F-83DF-04F29CD0984F}">
   <dimension ref="A1:P118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="G118" sqref="G118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2411,7 +2414,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2443,7 +2446,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2475,7 +2478,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2539,7 +2542,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2571,7 +2574,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2635,15 +2638,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>547</v>
       </c>
       <c r="D16" t="s">
         <v>40</v>
@@ -2667,7 +2670,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2731,7 +2734,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2763,7 +2766,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2795,7 +2798,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2827,7 +2830,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2862,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2891,7 +2894,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2923,7 +2926,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2955,7 +2958,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3019,7 +3022,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3051,7 +3054,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -3145,7 +3148,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -3192,7 +3195,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>123</v>
       </c>
@@ -3239,7 +3242,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>124</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>125</v>
       </c>
@@ -3333,7 +3336,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>126</v>
       </c>
@@ -3380,7 +3383,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -3430,7 +3433,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -3480,7 +3483,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -3530,7 +3533,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>130</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>131</v>
       </c>
@@ -3630,7 +3633,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>132</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>133</v>
       </c>
@@ -3730,7 +3733,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>134</v>
       </c>
@@ -3780,7 +3783,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>135</v>
       </c>
@@ -3830,7 +3833,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -3924,7 +3927,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -3971,7 +3974,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>138</v>
       </c>
@@ -4018,7 +4021,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>139</v>
       </c>
@@ -4068,7 +4071,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>140</v>
       </c>
@@ -4115,7 +4118,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -4162,7 +4165,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>142</v>
       </c>
@@ -4209,7 +4212,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>143</v>
       </c>
@@ -4256,7 +4259,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>144</v>
       </c>
@@ -4303,7 +4306,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>145</v>
       </c>
@@ -4350,7 +4353,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>146</v>
       </c>
@@ -4397,7 +4400,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>147</v>
       </c>
@@ -4444,7 +4447,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>148</v>
       </c>
@@ -4491,7 +4494,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>149</v>
       </c>
@@ -4538,7 +4541,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>150</v>
       </c>
@@ -4585,7 +4588,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>151</v>
       </c>
@@ -4632,7 +4635,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>152</v>
       </c>
@@ -4679,7 +4682,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>153</v>
       </c>
@@ -4726,7 +4729,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>154</v>
       </c>
@@ -4773,7 +4776,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>155</v>
       </c>
@@ -4823,7 +4826,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>156</v>
       </c>
@@ -4873,7 +4876,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>158</v>
       </c>
@@ -4920,7 +4923,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>159</v>
       </c>
@@ -4967,7 +4970,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>160</v>
       </c>
@@ -5014,7 +5017,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>161</v>
       </c>
@@ -5061,7 +5064,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>162</v>
       </c>
@@ -5108,7 +5111,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>163</v>
       </c>
@@ -5158,7 +5161,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>164</v>
       </c>
@@ -5205,7 +5208,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>165</v>
       </c>
@@ -5252,7 +5255,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>166</v>
       </c>
@@ -5299,7 +5302,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>167</v>
       </c>
@@ -5346,7 +5349,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>168</v>
       </c>
@@ -5393,7 +5396,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>169</v>
       </c>
@@ -5440,7 +5443,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>157</v>
       </c>
@@ -5490,7 +5493,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -5537,7 +5540,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>171</v>
       </c>
@@ -5584,7 +5587,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>172</v>
       </c>
@@ -5631,7 +5634,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -5678,7 +5681,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>174</v>
       </c>
@@ -5725,7 +5728,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>175</v>
       </c>
@@ -5772,7 +5775,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>176</v>
       </c>
@@ -5819,7 +5822,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -5866,7 +5869,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>178</v>
       </c>
@@ -5913,7 +5916,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>179</v>
       </c>
@@ -5960,7 +5963,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>341</v>
       </c>
@@ -6007,7 +6010,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -6054,7 +6057,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>181</v>
       </c>
@@ -6101,7 +6104,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -6148,7 +6151,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -6198,7 +6201,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>184</v>
       </c>
@@ -6245,7 +6248,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>185</v>
       </c>
@@ -6292,7 +6295,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>186</v>
       </c>
@@ -6339,7 +6342,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>187</v>
       </c>
@@ -6386,7 +6389,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>188</v>
       </c>
@@ -6433,7 +6436,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>189</v>
       </c>
@@ -6483,7 +6486,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>190</v>
       </c>
@@ -6533,7 +6536,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>191</v>
       </c>
@@ -6583,7 +6586,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>192</v>
       </c>
@@ -6633,7 +6636,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -6683,7 +6686,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>194</v>
       </c>
@@ -6733,7 +6736,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>195</v>
       </c>
@@ -6780,7 +6783,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>196</v>
       </c>
@@ -6827,7 +6830,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>340</v>
       </c>
@@ -6874,7 +6877,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>197</v>
       </c>
@@ -6921,7 +6924,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>198</v>
       </c>
@@ -6968,7 +6971,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>199</v>
       </c>
@@ -7015,7 +7018,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>200</v>
       </c>
@@ -7062,7 +7065,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>201</v>
       </c>
@@ -7109,7 +7112,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>202</v>
       </c>
@@ -7159,7 +7162,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>203</v>
       </c>
@@ -7209,7 +7212,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>204</v>
       </c>
@@ -7256,7 +7259,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>205</v>
       </c>
@@ -7300,7 +7303,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>175</v>
       </c>

</xml_diff>